<commit_message>
Change column order for easier  answer expansion
</commit_message>
<xml_diff>
--- a/docs/infosec-example.xlsx
+++ b/docs/infosec-example.xlsx
@@ -29,22 +29,22 @@
     <t xml:space="preserve">Question</t>
   </si>
   <si>
+    <t xml:space="preserve">Solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartSet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficulty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slope</t>
+  </si>
+  <si>
     <t xml:space="preserve">A1</t>
   </si>
   <si>
     <t xml:space="preserve">A2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartSet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Difficulty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slope</t>
   </si>
   <si>
     <t xml:space="preserve">Which of the following schemes is better for pasword creation?</t>
@@ -386,7 +386,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -408,19 +408,20 @@
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I:I"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="103.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="65.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="71.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="13.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="2" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="2" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="69.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="70.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -456,16 +457,16 @@
       <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -474,14 +475,14 @@
       <c r="B3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,16 +492,16 @@
       <c r="B4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -509,14 +510,14 @@
       <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,14 +527,16 @@
       <c r="B6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="b">
+      <c r="C6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,14 +546,14 @@
       <c r="B7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -560,14 +563,14 @@
       <c r="B8" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,14 +580,14 @@
       <c r="B9" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,14 +597,14 @@
       <c r="B10" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -611,14 +614,14 @@
       <c r="B11" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,14 +631,16 @@
       <c r="B12" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5" t="b">
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -645,14 +650,16 @@
       <c r="B13" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="5" t="b">
+      <c r="C13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -662,14 +669,14 @@
       <c r="B14" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="H14" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,14 +686,14 @@
       <c r="B15" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="H15" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -696,14 +703,16 @@
       <c r="B16" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" s="5" t="b">
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,14 +722,14 @@
       <c r="B17" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="H17" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -730,14 +739,14 @@
       <c r="B18" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,31 +756,33 @@
       <c r="B19" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5" t="b">
+      <c r="C19" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E19" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="H20" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,14 +792,14 @@
       <c r="B21" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="H21" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,14 +809,14 @@
       <c r="B22" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="H22" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,14 +826,14 @@
       <c r="B23" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="H23" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E23" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -832,14 +843,14 @@
       <c r="B24" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="H24" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -849,14 +860,14 @@
       <c r="B25" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="H25" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,14 +877,14 @@
       <c r="B26" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="H26" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -883,14 +894,14 @@
       <c r="B27" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="H27" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -900,14 +911,14 @@
       <c r="B28" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="H28" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -917,14 +928,14 @@
       <c r="B29" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="H29" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -934,14 +945,14 @@
       <c r="B30" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="H30" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -962,13 +973,13 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="I:I B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Mock difficulty, slope and start set for infosec
</commit_message>
<xml_diff>
--- a/docs/infosec-example.xlsx
+++ b/docs/infosec-example.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -47,7 +47,7 @@
     <t xml:space="preserve">A2</t>
   </si>
   <si>
-    <t xml:space="preserve">Which of the following schemes is better for pasword creation?</t>
+    <t xml:space="preserve">Which of the following schemes is better for password creation?</t>
   </si>
   <si>
     <t xml:space="preserve">Replacing characters with look-alike numbers or symbols</t>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t xml:space="preserve">How are most viruses distributed?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">Email</t>
@@ -329,12 +332,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -356,12 +358,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -406,7 +402,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -419,46 +415,42 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="103.51"/>
@@ -468,6 +460,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="9.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,7 +499,12 @@
       <c r="C2" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="E2" s="0" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>2.1</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
@@ -523,6 +521,12 @@
       </c>
       <c r="C3" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>2.09</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
@@ -541,29 +545,43 @@
       <c r="C4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1.85</v>
+      </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="E5" s="0" t="n">
+        <v>2.97</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>2.78</v>
+      </c>
       <c r="G5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,16 +589,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="E6" s="0" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="G6" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H6" s="5" t="n">
+      <c r="H6" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -590,16 +614,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="E7" s="0" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2.06</v>
+      </c>
       <c r="G7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,16 +637,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="E8" s="0" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>2.14</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -624,16 +660,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="E9" s="0" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>2.74</v>
+      </c>
       <c r="G9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,16 +683,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="E10" s="0" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>2.96</v>
+      </c>
       <c r="G10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,16 +706,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="E11" s="0" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>2.56</v>
+      </c>
       <c r="G11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,16 +729,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G12" s="5" t="n">
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="G12" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H12" s="5" t="n">
+      <c r="H12" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -694,16 +757,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G13" s="5" t="n">
+      <c r="E13" s="0" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>2.89</v>
+      </c>
+      <c r="G13" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H13" s="5" t="n">
+      <c r="H13" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -713,16 +782,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="E14" s="0" t="n">
+        <v>-0.56</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>2.04</v>
+      </c>
       <c r="G14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -730,16 +805,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="E15" s="0" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>2.55</v>
+      </c>
       <c r="G15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,16 +828,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G16" s="5" t="n">
+      <c r="E16" s="0" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="G16" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H16" s="5" t="n">
+      <c r="H16" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -766,16 +853,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="E17" s="0" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>2.24</v>
+      </c>
       <c r="G17" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,16 +876,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="E18" s="0" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>2.22</v>
+      </c>
       <c r="G18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -800,35 +899,47 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G19" s="5" t="n">
+      <c r="E19" s="0" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="G19" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H19" s="5" t="n">
+      <c r="H19" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="35.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="36.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>52</v>
+      <c r="B20" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="E20" s="0" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>1.72</v>
+      </c>
       <c r="G20" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -836,16 +947,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1.12</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,16 +970,25 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="D22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>2.33</v>
+      </c>
       <c r="G22" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -870,16 +996,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="E23" s="0" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>1.26</v>
+      </c>
       <c r="G23" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,16 +1019,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="E24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>1.63</v>
+      </c>
       <c r="G24" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,16 +1042,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="E25" s="0" t="n">
+        <v>-0.93</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>1.88</v>
+      </c>
       <c r="G25" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -921,16 +1065,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="E26" s="0" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>2.98</v>
+      </c>
       <c r="G26" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,16 +1088,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="E27" s="0" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>1.32</v>
+      </c>
       <c r="G27" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -955,16 +1111,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="E28" s="0" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>2.31</v>
+      </c>
       <c r="G28" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -972,16 +1134,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="E29" s="0" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>1.49</v>
+      </c>
       <c r="G29" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -989,16 +1157,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="E30" s="0" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>1.32</v>
+      </c>
       <c r="G30" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,16 +1180,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="E31" s="0" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>1.28</v>
+      </c>
       <c r="G31" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,16 +1203,22 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="E32" s="0" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>1.39</v>
+      </c>
       <c r="G32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H32" s="6" t="s">
         <v>90</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,16 +1226,22 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G33" s="4" t="s">
-        <v>92</v>
+      <c r="E33" s="0" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1057,16 +1249,22 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="E34" s="0" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>2.68</v>
+      </c>
       <c r="G34" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1081,7 +1279,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1091,23 +1289,24 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>16</v>

</xml_diff>

<commit_message>
BugFix: Duplicate Submits were not prohibited
@Flo
</commit_message>
<xml_diff>
--- a/docs/infosec-example.xlsx
+++ b/docs/infosec-example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\repos\satoca\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekte\satoca\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95C7E4F-DEE9-4737-9A86-4AFE9B88B632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909FEB37-F819-4BD0-A55E-E0F0A7493861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>Item severity boundary</t>
+  </si>
+  <si>
+    <t>Privacy Budget</t>
   </si>
 </sst>
 </file>
@@ -1561,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,6 +1601,14 @@
         <v>0.05</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4">
+        <v>0.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Revert "Feature/display errors to participant"
</commit_message>
<xml_diff>
--- a/docs/infosec-example.xlsx
+++ b/docs/infosec-example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekte\satoca\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\repos\satoca\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909FEB37-F819-4BD0-A55E-E0F0A7493861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95C7E4F-DEE9-4737-9A86-4AFE9B88B632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="105">
   <si>
     <t>ID</t>
   </si>
@@ -352,9 +352,6 @@
   </si>
   <si>
     <t>Item severity boundary</t>
-  </si>
-  <si>
-    <t>Privacy Budget</t>
   </si>
 </sst>
 </file>
@@ -1564,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,14 +1598,6 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4">
-        <v>0.8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Add privacy budget to infosec-example
</commit_message>
<xml_diff>
--- a/docs/infosec-example.xlsx
+++ b/docs/infosec-example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\repos\satoca\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95C7E4F-DEE9-4737-9A86-4AFE9B88B632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A700F3-0224-4963-8670-42C41AA7D802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>Item severity boundary</t>
+  </si>
+  <si>
+    <t>Privacy Budget</t>
   </si>
 </sst>
 </file>
@@ -1561,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,8 +1601,16 @@
         <v>0.05</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>